<commit_message>
using filter to have dynamic charts:: by sergio giraldo @ 20230311T1726CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/DynamicCharts.xlsx
+++ b/excel/DynamicCharts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC160601-82F5-2F41-A017-3071FDEB6572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B6B3E4-1098-C740-B015-5DE818559146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{2193EDC7-304B-DB4E-9D6F-D7AE1DC66F88}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>Department</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>To</t>
+  </si>
+  <si>
+    <t>&lt;- Change this and the chart updates automagically</t>
+  </si>
+  <si>
+    <t>&lt;- Change the range of data and the chart updates automagically</t>
   </si>
 </sst>
 </file>
@@ -265,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -321,12 +327,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -340,6 +357,10 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -919,168 +940,48 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$39:$E$63</c:f>
+              <c:f>Sheet1!$E$39:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>44959</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>44960</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>44961</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>44962</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>44963</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44964</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44965</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44966</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44967</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44968</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44969</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44970</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44971</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44972</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44973</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44974</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44975</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44976</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44977</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44978</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44979</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44980</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44981</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44982</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44983</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$39:$F$63</c:f>
+              <c:f>Sheet1!$F$39:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>47571</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>66219</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>83371</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>25825</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>24740</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>79865</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>31997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>50260</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>59470</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>83073</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89815</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>27757</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>96261</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>79856</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>34517</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49383</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>95541</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>71984</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>71215</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>93955</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>30916</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>65780</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>99047</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>32910</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>31381</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>80763</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2474,7 +2375,7 @@
     <tableColumn id="2" xr3:uid="{44E203C1-AA34-6E41-8036-064F1489E91F}" name="Name" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{BBCA9883-28BB-3141-805B-11929FF17B6B}" name="Amount" dataDxfId="2" dataCellStyle="Comma"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2788,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA34215A-BC5C-B24D-AE21-1B1A62ABDCFB}">
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2829,6 +2730,9 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -3260,11 +3164,14 @@
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="10">
-        <v>44959</v>
+        <v>44958</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -3274,11 +3181,11 @@
       <c r="B36" s="7">
         <v>89303</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="11" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="9">
-        <v>44985</v>
+        <v>44964</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -3311,11 +3218,11 @@
         <v>83371</v>
       </c>
       <c r="E39" s="9" cm="1">
-        <f t="array" ref="E39:F63">_xlfn._xlws.FILTER(Table2[],(Table2[Date]&gt;D35)*(Table2[Date]&lt;D36))</f>
-        <v>44960</v>
+        <f t="array" ref="E39:F43">_xlfn._xlws.FILTER(Table2[],(Table2[Date]&gt;D35)*(Table2[Date]&lt;D36))</f>
+        <v>44959</v>
       </c>
       <c r="F39" s="2">
-        <v>66219</v>
+        <v>47571</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -3326,10 +3233,10 @@
         <v>25825</v>
       </c>
       <c r="E40" s="9">
-        <v>44961</v>
+        <v>44960</v>
       </c>
       <c r="F40" s="2">
-        <v>83371</v>
+        <v>66219</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3340,10 +3247,10 @@
         <v>24740</v>
       </c>
       <c r="E41" s="9">
-        <v>44962</v>
+        <v>44961</v>
       </c>
       <c r="F41" s="2">
-        <v>25825</v>
+        <v>83371</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3354,10 +3261,10 @@
         <v>79865</v>
       </c>
       <c r="E42" s="9">
-        <v>44963</v>
+        <v>44962</v>
       </c>
       <c r="F42" s="2">
-        <v>24740</v>
+        <v>25825</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3368,10 +3275,10 @@
         <v>31997</v>
       </c>
       <c r="E43" s="9">
-        <v>44964</v>
+        <v>44963</v>
       </c>
       <c r="F43" s="2">
-        <v>79865</v>
+        <v>24740</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3381,12 +3288,8 @@
       <c r="B44" s="7">
         <v>50260</v>
       </c>
-      <c r="E44" s="9">
-        <v>44965</v>
-      </c>
-      <c r="F44" s="2">
-        <v>31997</v>
-      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
@@ -3395,12 +3298,8 @@
       <c r="B45" s="7">
         <v>59470</v>
       </c>
-      <c r="E45" s="9">
-        <v>44966</v>
-      </c>
-      <c r="F45" s="2">
-        <v>50260</v>
-      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
@@ -3409,12 +3308,8 @@
       <c r="B46" s="7">
         <v>83073</v>
       </c>
-      <c r="E46" s="9">
-        <v>44967</v>
-      </c>
-      <c r="F46" s="2">
-        <v>59470</v>
-      </c>
+      <c r="E46" s="9"/>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
@@ -3423,12 +3318,8 @@
       <c r="B47" s="7">
         <v>89815</v>
       </c>
-      <c r="E47" s="9">
-        <v>44968</v>
-      </c>
-      <c r="F47" s="2">
-        <v>83073</v>
-      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
@@ -3437,12 +3328,8 @@
       <c r="B48" s="7">
         <v>27757</v>
       </c>
-      <c r="E48" s="9">
-        <v>44969</v>
-      </c>
-      <c r="F48" s="2">
-        <v>89815</v>
-      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
@@ -3451,12 +3338,8 @@
       <c r="B49" s="7">
         <v>96261</v>
       </c>
-      <c r="E49" s="9">
-        <v>44970</v>
-      </c>
-      <c r="F49" s="2">
-        <v>27757</v>
-      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
@@ -3465,12 +3348,8 @@
       <c r="B50" s="7">
         <v>79856</v>
       </c>
-      <c r="E50" s="9">
-        <v>44971</v>
-      </c>
-      <c r="F50" s="2">
-        <v>96261</v>
-      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
@@ -3479,12 +3358,8 @@
       <c r="B51" s="7">
         <v>34517</v>
       </c>
-      <c r="E51" s="9">
-        <v>44972</v>
-      </c>
-      <c r="F51" s="2">
-        <v>79856</v>
-      </c>
+      <c r="E51" s="9"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
@@ -3493,12 +3368,8 @@
       <c r="B52" s="7">
         <v>49383</v>
       </c>
-      <c r="E52" s="9">
-        <v>44973</v>
-      </c>
-      <c r="F52" s="2">
-        <v>34517</v>
-      </c>
+      <c r="E52" s="9"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
@@ -3507,12 +3378,8 @@
       <c r="B53" s="7">
         <v>95541</v>
       </c>
-      <c r="E53" s="9">
-        <v>44974</v>
-      </c>
-      <c r="F53" s="2">
-        <v>49383</v>
-      </c>
+      <c r="E53" s="9"/>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
@@ -3521,12 +3388,8 @@
       <c r="B54" s="7">
         <v>71984</v>
       </c>
-      <c r="E54" s="9">
-        <v>44975</v>
-      </c>
-      <c r="F54" s="2">
-        <v>95541</v>
-      </c>
+      <c r="E54" s="9"/>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
@@ -3535,12 +3398,8 @@
       <c r="B55" s="7">
         <v>71215</v>
       </c>
-      <c r="E55" s="9">
-        <v>44976</v>
-      </c>
-      <c r="F55" s="2">
-        <v>71984</v>
-      </c>
+      <c r="E55" s="9"/>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
@@ -3549,12 +3408,8 @@
       <c r="B56" s="7">
         <v>93955</v>
       </c>
-      <c r="E56" s="9">
-        <v>44977</v>
-      </c>
-      <c r="F56" s="2">
-        <v>71215</v>
-      </c>
+      <c r="E56" s="9"/>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
@@ -3563,12 +3418,8 @@
       <c r="B57" s="7">
         <v>30916</v>
       </c>
-      <c r="E57" s="9">
-        <v>44978</v>
-      </c>
-      <c r="F57" s="2">
-        <v>93955</v>
-      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
@@ -3577,12 +3428,8 @@
       <c r="B58" s="7">
         <v>65780</v>
       </c>
-      <c r="E58" s="9">
-        <v>44979</v>
-      </c>
-      <c r="F58" s="2">
-        <v>30916</v>
-      </c>
+      <c r="E58" s="9"/>
+      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
@@ -3591,12 +3438,8 @@
       <c r="B59" s="7">
         <v>99047</v>
       </c>
-      <c r="E59" s="9">
-        <v>44980</v>
-      </c>
-      <c r="F59" s="2">
-        <v>65780</v>
-      </c>
+      <c r="E59" s="9"/>
+      <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
@@ -3605,12 +3448,8 @@
       <c r="B60" s="7">
         <v>32910</v>
       </c>
-      <c r="E60" s="9">
-        <v>44981</v>
-      </c>
-      <c r="F60" s="2">
-        <v>99047</v>
-      </c>
+      <c r="E60" s="9"/>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
@@ -3619,12 +3458,8 @@
       <c r="B61" s="7">
         <v>31381</v>
       </c>
-      <c r="E61" s="9">
-        <v>44982</v>
-      </c>
-      <c r="F61" s="2">
-        <v>32910</v>
-      </c>
+      <c r="E61" s="9"/>
+      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
@@ -3633,12 +3468,8 @@
       <c r="B62" s="7">
         <v>80763</v>
       </c>
-      <c r="E62" s="9">
-        <v>44983</v>
-      </c>
-      <c r="F62" s="2">
-        <v>31381</v>
-      </c>
+      <c r="E62" s="9"/>
+      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
@@ -3647,12 +3478,8 @@
       <c r="B63" s="7">
         <v>39088</v>
       </c>
-      <c r="E63" s="9">
-        <v>44984</v>
-      </c>
-      <c r="F63" s="2">
-        <v>80763</v>
-      </c>
+      <c r="E63" s="9"/>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
@@ -3678,7 +3505,7 @@
       <c r="A66" s="9">
         <v>44988</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="2">
         <v>55107</v>
       </c>
       <c r="E66" s="9"/>
@@ -3688,7 +3515,7 @@
       <c r="A67" s="9">
         <v>44989</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="12">
         <v>60348</v>
       </c>
       <c r="E67" s="9"/>
@@ -3698,7 +3525,7 @@
       <c r="A68" s="9">
         <v>44990</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="2">
         <v>72298</v>
       </c>
       <c r="E68" s="9"/>
@@ -3708,7 +3535,7 @@
       <c r="A69" s="9">
         <v>44991</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="12">
         <v>69721</v>
       </c>
       <c r="E69" s="9"/>
@@ -3718,7 +3545,7 @@
       <c r="A70" s="9">
         <v>44992</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="2">
         <v>61125</v>
       </c>
       <c r="E70" s="9"/>
@@ -3728,7 +3555,7 @@
       <c r="A71" s="9">
         <v>44993</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="12">
         <v>79270</v>
       </c>
       <c r="E71" s="9"/>
@@ -3738,7 +3565,7 @@
       <c r="A72" s="9">
         <v>44994</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="2">
         <v>45347</v>
       </c>
       <c r="E72" s="9"/>
@@ -3748,7 +3575,7 @@
       <c r="A73" s="9">
         <v>44995</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="12">
         <v>46243</v>
       </c>
       <c r="E73" s="9"/>
@@ -3758,7 +3585,7 @@
       <c r="A74" s="9">
         <v>44996</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="2">
         <v>77384</v>
       </c>
       <c r="E74" s="9"/>
@@ -3768,7 +3595,7 @@
       <c r="A75" s="9">
         <v>44997</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="12">
         <v>55917</v>
       </c>
       <c r="E75" s="9"/>
@@ -3778,7 +3605,7 @@
       <c r="A76" s="9">
         <v>44998</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="2">
         <v>57507</v>
       </c>
       <c r="E76" s="9"/>
@@ -3788,7 +3615,7 @@
       <c r="A77" s="9">
         <v>44999</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="12">
         <v>53797</v>
       </c>
       <c r="E77" s="9"/>
@@ -3798,7 +3625,7 @@
       <c r="A78" s="9">
         <v>45000</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="2">
         <v>73461</v>
       </c>
       <c r="E78" s="9"/>
@@ -3808,7 +3635,7 @@
       <c r="A79" s="9">
         <v>45001</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="12">
         <v>45694</v>
       </c>
       <c r="E79" s="9"/>
@@ -3818,7 +3645,7 @@
       <c r="A80" s="9">
         <v>45002</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="2">
         <v>61866</v>
       </c>
       <c r="E80" s="9"/>
@@ -3828,7 +3655,7 @@
       <c r="A81" s="9">
         <v>45003</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="12">
         <v>33286</v>
       </c>
       <c r="E81" s="9"/>
@@ -3838,7 +3665,7 @@
       <c r="A82" s="9">
         <v>45004</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="2">
         <v>31087</v>
       </c>
       <c r="E82" s="9"/>
@@ -3848,7 +3675,7 @@
       <c r="A83" s="9">
         <v>45005</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="12">
         <v>52874</v>
       </c>
       <c r="E83" s="9"/>
@@ -3858,7 +3685,7 @@
       <c r="A84" s="9">
         <v>45006</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="2">
         <v>39942</v>
       </c>
       <c r="E84" s="9"/>
@@ -3868,7 +3695,7 @@
       <c r="A85" s="9">
         <v>45007</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="12">
         <v>59000</v>
       </c>
       <c r="E85" s="9"/>
@@ -3878,7 +3705,7 @@
       <c r="A86" s="9">
         <v>45008</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="2">
         <v>51423</v>
       </c>
       <c r="E86" s="9"/>
@@ -3888,7 +3715,7 @@
       <c r="A87" s="9">
         <v>45009</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="12">
         <v>57857</v>
       </c>
       <c r="E87" s="9"/>
@@ -3898,7 +3725,7 @@
       <c r="A88" s="9">
         <v>45010</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="2">
         <v>76193</v>
       </c>
       <c r="E88" s="9"/>
@@ -3908,7 +3735,7 @@
       <c r="A89" s="9">
         <v>45011</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="12">
         <v>70551</v>
       </c>
       <c r="E89" s="9"/>
@@ -3918,7 +3745,7 @@
       <c r="A90" s="9">
         <v>45012</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="2">
         <v>74145</v>
       </c>
       <c r="E90" s="9"/>
@@ -3928,7 +3755,7 @@
       <c r="A91" s="9">
         <v>45013</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="12">
         <v>79181</v>
       </c>
       <c r="E91" s="9"/>
@@ -3938,7 +3765,7 @@
       <c r="A92" s="9">
         <v>45014</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="2">
         <v>63917</v>
       </c>
       <c r="E92" s="9"/>
@@ -3948,7 +3775,7 @@
       <c r="A93" s="9">
         <v>45015</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="12">
         <v>74700</v>
       </c>
       <c r="E93" s="9"/>
@@ -3958,7 +3785,7 @@
       <c r="A94" s="9">
         <v>45016</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="2">
         <v>71584</v>
       </c>
       <c r="E94" s="9"/>

</xml_diff>

<commit_message>
using filter to have dynamic charts:: by sergio giraldo @ 20230311T1735CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/DynamicCharts.xlsx
+++ b/excel/DynamicCharts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B6B3E4-1098-C740-B015-5DE818559146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB080E2B-F78B-2640-9CC3-3CE7EB19C1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{2193EDC7-304B-DB4E-9D6F-D7AE1DC66F88}"/>
   </bookViews>
@@ -37,9 +37,8 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+  <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -50,25 +49,11 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-  </valueMetadata>
 </metadata>
 </file>
 
@@ -558,77 +543,47 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$5:$F$14</c:f>
+              <c:f>Sheet1!$F$5:$F$9</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>james</c:v>
+                  <c:v>jamille</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>jeb</c:v>
+                  <c:v>jeremiah</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>jeff</c:v>
+                  <c:v>jethro</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>jill</c:v>
+                  <c:v>june</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>jonas</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>judas</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>marvin</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>michael</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>mitch</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>monica</c:v>
+                  <c:v>molly</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$14</c:f>
+              <c:f>Sheet1!$G$5:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25825</c:v>
+                  <c:v>79856</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49383</c:v>
+                  <c:v>27757</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79865</c:v>
+                  <c:v>96261</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83371</c:v>
+                  <c:v>34517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24740</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>71984</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>31381</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>65780</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>99047</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>32910</c:v>
+                  <c:v>66537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -863,7 +818,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$38</c:f>
+              <c:f>Sheet1!$F$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -940,48 +895,168 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$39:$E$43</c:f>
+              <c:f>Sheet1!$E$39:$E$63</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>44959</c:v>
+                  <c:v>44961</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44960</c:v>
+                  <c:v>44962</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44961</c:v>
+                  <c:v>44963</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44962</c:v>
+                  <c:v>44964</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44963</c:v>
+                  <c:v>44965</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44966</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44968</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44969</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44970</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44971</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44972</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44973</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44974</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44975</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44976</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44977</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44978</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44979</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44980</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44981</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44982</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44983</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44984</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$39:$F$43</c:f>
+              <c:f>Sheet1!$F$39:$F$63</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>47571</c:v>
+                  <c:v>83371</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66219</c:v>
+                  <c:v>25825</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83371</c:v>
+                  <c:v>24740</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25825</c:v>
+                  <c:v>79865</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24740</c:v>
+                  <c:v>31997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50260</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59470</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83073</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89815</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27757</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>96261</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>79856</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34517</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49383</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95541</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>71984</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>71215</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>93955</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30916</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>65780</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99047</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32910</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31381</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80763</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39088</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2233,15 +2308,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:colOff>787400</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2270,13 +2345,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2305,68 +2380,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>0</v>
-    <v>8</v>
-    <v>3</v>
-    <v>6</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_error">
-    <k n="colOffset" t="i"/>
-    <k n="errorType" t="i"/>
-    <k n="rwOffset" t="i"/>
-    <k n="subType" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6EED9968-2614-0845-A707-A4401A456C35}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C31" xr:uid="{6EED9968-2614-0845-A707-A4401A456C35}"/>
@@ -2380,8 +2393,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43A57240-965E-1A43-9BDD-0FBA2394B7CD}" name="Table2" displayName="Table2" ref="A35:B94" totalsRowShown="0">
-  <autoFilter ref="A35:B94" xr:uid="{43A57240-965E-1A43-9BDD-0FBA2394B7CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{43A57240-965E-1A43-9BDD-0FBA2394B7CD}" name="Table2" displayName="Table2" ref="A33:B92" totalsRowShown="0">
+  <autoFilter ref="A33:B92" xr:uid="{43A57240-965E-1A43-9BDD-0FBA2394B7CD}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A98A474F-896B-B842-862D-3CC234F16E72}" name="Date" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{1DD1586F-8704-314C-9B4C-8B2CFA0C7C65}" name="Amount" dataDxfId="1"/>
@@ -2687,10 +2700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA34215A-BC5C-B24D-AE21-1B1A62ABDCFB}">
-  <dimension ref="A1:S94"/>
+  <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2728,7 +2741,7 @@
         <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>41</v>
@@ -2744,10 +2757,7 @@
       <c r="C3" s="2">
         <v>47571</v>
       </c>
-      <c r="S3" s="4" t="e" cm="1" vm="1">
-        <f t="array" aca="1" ref="S3" ca="1">_xlfn.UNIQUE(Table1[Department])</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2767,7 +2777,7 @@
       </c>
       <c r="I4" s="6" t="str">
         <f>G2</f>
-        <v>Sales</v>
+        <v>Procurement</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -2791,11 +2801,11 @@
         <v>83371</v>
       </c>
       <c r="F5" s="1" t="str" cm="1">
-        <f t="array" ref="F5:G14">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(Table1[[Name]:[Amount]],Table1[Department]=G2))</f>
-        <v>james</v>
+        <f t="array" ref="F5:G9">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(Table1[[Name]:[Amount]],Table1[Department]=G2))</f>
+        <v>jamille</v>
       </c>
       <c r="G5" s="5">
-        <v>25825</v>
+        <v>79856</v>
       </c>
       <c r="S5" s="4"/>
     </row>
@@ -2810,10 +2820,14 @@
         <v>25825</v>
       </c>
       <c r="F6" s="1" t="str">
-        <v>jeb</v>
+        <v>jeremiah</v>
       </c>
       <c r="G6" s="5">
-        <v>49383</v>
+        <v>27757</v>
+      </c>
+      <c r="I6" s="1" t="str" cm="1">
+        <f t="array" ref="I6:I9">_xlfn.UNIQUE(Table1[Department])</f>
+        <v>Finance</v>
       </c>
       <c r="S6" s="4"/>
     </row>
@@ -2828,10 +2842,13 @@
         <v>24740</v>
       </c>
       <c r="F7" s="1" t="str">
-        <v>jeff</v>
+        <v>jethro</v>
       </c>
       <c r="G7" s="5">
-        <v>79865</v>
+        <v>96261</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <v>Sales</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2845,10 +2862,13 @@
         <v>79865</v>
       </c>
       <c r="F8" s="1" t="str">
-        <v>jill</v>
+        <v>june</v>
       </c>
       <c r="G8" s="5">
-        <v>83371</v>
+        <v>34517</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <v>Compliance</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2862,10 +2882,13 @@
         <v>31997</v>
       </c>
       <c r="F9" s="1" t="str">
-        <v>jonas</v>
+        <v>molly</v>
       </c>
       <c r="G9" s="5">
-        <v>24740</v>
+        <v>66537</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <v>Procurement</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -2878,12 +2901,7 @@
       <c r="C10" s="2">
         <v>50260</v>
       </c>
-      <c r="F10" s="1" t="str">
-        <v>judas</v>
-      </c>
-      <c r="G10" s="5">
-        <v>71984</v>
-      </c>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2895,12 +2913,7 @@
       <c r="C11" s="2">
         <v>59470</v>
       </c>
-      <c r="F11" s="1" t="str">
-        <v>marvin</v>
-      </c>
-      <c r="G11" s="5">
-        <v>31381</v>
-      </c>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2912,12 +2925,7 @@
       <c r="C12" s="2">
         <v>83073</v>
       </c>
-      <c r="F12" s="1" t="str">
-        <v>michael</v>
-      </c>
-      <c r="G12" s="5">
-        <v>65780</v>
-      </c>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -2929,12 +2937,7 @@
       <c r="C13" s="2">
         <v>89815</v>
       </c>
-      <c r="F13" s="1" t="str">
-        <v>mitch</v>
-      </c>
-      <c r="G13" s="5">
-        <v>99047</v>
-      </c>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -2946,12 +2949,7 @@
       <c r="C14" s="2">
         <v>27757</v>
       </c>
-      <c r="F14" s="1" t="str">
-        <v>monica</v>
-      </c>
-      <c r="G14" s="5">
-        <v>32910</v>
-      </c>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -3157,647 +3155,735 @@
       </c>
       <c r="G31" s="5"/>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="10">
+        <v>44958</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>44958</v>
+      </c>
+      <c r="B34" s="7">
+        <v>89303</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="9">
+        <v>44986</v>
+      </c>
+    </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="10">
-        <v>44958</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>42</v>
+      <c r="A35" s="9">
+        <v>44959</v>
+      </c>
+      <c r="B35" s="7">
+        <v>47571</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
-        <v>44958</v>
+        <v>44960</v>
       </c>
       <c r="B36" s="7">
-        <v>89303</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="9">
-        <v>44964</v>
+        <v>66219</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
+        <v>44961</v>
+      </c>
+      <c r="B37" s="7">
+        <v>83371</v>
+      </c>
+      <c r="E37" s="9" cm="1">
+        <f t="array" ref="E37:F63">_xlfn._xlws.FILTER(Table2[],(Table2[Date]&gt;D33)*(Table2[Date]&lt;D34))</f>
         <v>44959</v>
       </c>
-      <c r="B37" s="7">
+      <c r="F37" s="2">
         <v>47571</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
+        <v>44962</v>
+      </c>
+      <c r="B38" s="7">
+        <v>25825</v>
+      </c>
+      <c r="E38" s="9">
         <v>44960</v>
       </c>
-      <c r="B38" s="7">
+      <c r="F38" s="2">
         <v>66219</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
+        <v>44963</v>
+      </c>
+      <c r="B39" s="7">
+        <v>24740</v>
+      </c>
+      <c r="E39" s="9">
         <v>44961</v>
       </c>
-      <c r="B39" s="7">
+      <c r="F39" s="2">
         <v>83371</v>
-      </c>
-      <c r="E39" s="9" cm="1">
-        <f t="array" ref="E39:F43">_xlfn._xlws.FILTER(Table2[],(Table2[Date]&gt;D35)*(Table2[Date]&lt;D36))</f>
-        <v>44959</v>
-      </c>
-      <c r="F39" s="2">
-        <v>47571</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
+        <v>44964</v>
+      </c>
+      <c r="B40" s="7">
+        <v>79865</v>
+      </c>
+      <c r="E40" s="9">
         <v>44962</v>
       </c>
-      <c r="B40" s="7">
+      <c r="F40" s="2">
         <v>25825</v>
-      </c>
-      <c r="E40" s="9">
-        <v>44960</v>
-      </c>
-      <c r="F40" s="2">
-        <v>66219</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
+        <v>44965</v>
+      </c>
+      <c r="B41" s="7">
+        <v>31997</v>
+      </c>
+      <c r="E41" s="9">
         <v>44963</v>
       </c>
-      <c r="B41" s="7">
+      <c r="F41" s="2">
         <v>24740</v>
-      </c>
-      <c r="E41" s="9">
-        <v>44961</v>
-      </c>
-      <c r="F41" s="2">
-        <v>83371</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
+        <v>44966</v>
+      </c>
+      <c r="B42" s="7">
+        <v>50260</v>
+      </c>
+      <c r="E42" s="9">
         <v>44964</v>
       </c>
-      <c r="B42" s="7">
+      <c r="F42" s="2">
         <v>79865</v>
-      </c>
-      <c r="E42" s="9">
-        <v>44962</v>
-      </c>
-      <c r="F42" s="2">
-        <v>25825</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
+        <v>44967</v>
+      </c>
+      <c r="B43" s="7">
+        <v>59470</v>
+      </c>
+      <c r="E43" s="9">
         <v>44965</v>
       </c>
-      <c r="B43" s="7">
+      <c r="F43" s="2">
         <v>31997</v>
-      </c>
-      <c r="E43" s="9">
-        <v>44963</v>
-      </c>
-      <c r="F43" s="2">
-        <v>24740</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
+        <v>44968</v>
+      </c>
+      <c r="B44" s="7">
+        <v>83073</v>
+      </c>
+      <c r="E44" s="9">
         <v>44966</v>
       </c>
-      <c r="B44" s="7">
+      <c r="F44" s="2">
         <v>50260</v>
       </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
+        <v>44969</v>
+      </c>
+      <c r="B45" s="7">
+        <v>89815</v>
+      </c>
+      <c r="E45" s="9">
         <v>44967</v>
       </c>
-      <c r="B45" s="7">
+      <c r="F45" s="2">
         <v>59470</v>
       </c>
-      <c r="E45" s="9"/>
-      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
+        <v>44970</v>
+      </c>
+      <c r="B46" s="7">
+        <v>27757</v>
+      </c>
+      <c r="E46" s="9">
         <v>44968</v>
       </c>
-      <c r="B46" s="7">
+      <c r="F46" s="2">
         <v>83073</v>
       </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
+        <v>44971</v>
+      </c>
+      <c r="B47" s="7">
+        <v>96261</v>
+      </c>
+      <c r="E47" s="9">
         <v>44969</v>
       </c>
-      <c r="B47" s="7">
+      <c r="F47" s="2">
         <v>89815</v>
       </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
+        <v>44972</v>
+      </c>
+      <c r="B48" s="7">
+        <v>79856</v>
+      </c>
+      <c r="E48" s="9">
         <v>44970</v>
       </c>
-      <c r="B48" s="7">
+      <c r="F48" s="2">
         <v>27757</v>
       </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
+        <v>44973</v>
+      </c>
+      <c r="B49" s="7">
+        <v>34517</v>
+      </c>
+      <c r="E49" s="9">
         <v>44971</v>
       </c>
-      <c r="B49" s="7">
+      <c r="F49" s="2">
         <v>96261</v>
       </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
+        <v>44974</v>
+      </c>
+      <c r="B50" s="7">
+        <v>49383</v>
+      </c>
+      <c r="E50" s="9">
         <v>44972</v>
       </c>
-      <c r="B50" s="7">
+      <c r="F50" s="2">
         <v>79856</v>
       </c>
-      <c r="E50" s="9"/>
-      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
+        <v>44975</v>
+      </c>
+      <c r="B51" s="7">
+        <v>95541</v>
+      </c>
+      <c r="E51" s="9">
         <v>44973</v>
       </c>
-      <c r="B51" s="7">
+      <c r="F51" s="2">
         <v>34517</v>
       </c>
-      <c r="E51" s="9"/>
-      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
+        <v>44976</v>
+      </c>
+      <c r="B52" s="7">
+        <v>71984</v>
+      </c>
+      <c r="E52" s="9">
         <v>44974</v>
       </c>
-      <c r="B52" s="7">
+      <c r="F52" s="2">
         <v>49383</v>
       </c>
-      <c r="E52" s="9"/>
-      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
+        <v>44977</v>
+      </c>
+      <c r="B53" s="7">
+        <v>71215</v>
+      </c>
+      <c r="E53" s="9">
         <v>44975</v>
       </c>
-      <c r="B53" s="7">
+      <c r="F53" s="2">
         <v>95541</v>
       </c>
-      <c r="E53" s="9"/>
-      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
+        <v>44978</v>
+      </c>
+      <c r="B54" s="7">
+        <v>93955</v>
+      </c>
+      <c r="E54" s="9">
         <v>44976</v>
       </c>
-      <c r="B54" s="7">
+      <c r="F54" s="2">
         <v>71984</v>
       </c>
-      <c r="E54" s="9"/>
-      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
+        <v>44979</v>
+      </c>
+      <c r="B55" s="7">
+        <v>30916</v>
+      </c>
+      <c r="E55" s="9">
         <v>44977</v>
       </c>
-      <c r="B55" s="7">
+      <c r="F55" s="2">
         <v>71215</v>
       </c>
-      <c r="E55" s="9"/>
-      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
+        <v>44980</v>
+      </c>
+      <c r="B56" s="7">
+        <v>65780</v>
+      </c>
+      <c r="E56" s="9">
         <v>44978</v>
       </c>
-      <c r="B56" s="7">
+      <c r="F56" s="2">
         <v>93955</v>
       </c>
-      <c r="E56" s="9"/>
-      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
+        <v>44981</v>
+      </c>
+      <c r="B57" s="7">
+        <v>99047</v>
+      </c>
+      <c r="E57" s="9">
         <v>44979</v>
       </c>
-      <c r="B57" s="7">
+      <c r="F57" s="2">
         <v>30916</v>
       </c>
-      <c r="E57" s="9"/>
-      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
+        <v>44982</v>
+      </c>
+      <c r="B58" s="7">
+        <v>32910</v>
+      </c>
+      <c r="E58" s="9">
         <v>44980</v>
       </c>
-      <c r="B58" s="7">
+      <c r="F58" s="2">
         <v>65780</v>
       </c>
-      <c r="E58" s="9"/>
-      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
+        <v>44983</v>
+      </c>
+      <c r="B59" s="7">
+        <v>31381</v>
+      </c>
+      <c r="E59" s="9">
         <v>44981</v>
       </c>
-      <c r="B59" s="7">
+      <c r="F59" s="2">
         <v>99047</v>
       </c>
-      <c r="E59" s="9"/>
-      <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
+        <v>44984</v>
+      </c>
+      <c r="B60" s="7">
+        <v>80763</v>
+      </c>
+      <c r="E60" s="9">
         <v>44982</v>
       </c>
-      <c r="B60" s="7">
+      <c r="F60" s="2">
         <v>32910</v>
       </c>
-      <c r="E60" s="9"/>
-      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
+        <v>44985</v>
+      </c>
+      <c r="B61" s="7">
+        <v>39088</v>
+      </c>
+      <c r="E61" s="9">
         <v>44983</v>
       </c>
-      <c r="B61" s="7">
+      <c r="F61" s="2">
         <v>31381</v>
       </c>
-      <c r="E61" s="9"/>
-      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
+        <v>44986</v>
+      </c>
+      <c r="B62" s="7">
+        <v>60758</v>
+      </c>
+      <c r="E62" s="9">
         <v>44984</v>
       </c>
-      <c r="B62" s="7">
+      <c r="F62" s="2">
         <v>80763</v>
       </c>
-      <c r="E62" s="9"/>
-      <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
+        <v>44987</v>
+      </c>
+      <c r="B63" s="8">
+        <v>66537</v>
+      </c>
+      <c r="E63" s="9">
         <v>44985</v>
       </c>
-      <c r="B63" s="7">
+      <c r="F63" s="2">
         <v>39088</v>
       </c>
-      <c r="E63" s="9"/>
-      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
-        <v>44986</v>
-      </c>
-      <c r="B64" s="7">
-        <v>60758</v>
+        <v>44988</v>
+      </c>
+      <c r="B64" s="2">
+        <v>55107</v>
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
-        <v>44987</v>
-      </c>
-      <c r="B65" s="8">
-        <v>66537</v>
+        <v>44989</v>
+      </c>
+      <c r="B65" s="12">
+        <v>60348</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
-        <v>44988</v>
+        <v>44990</v>
       </c>
       <c r="B66" s="2">
-        <v>55107</v>
+        <v>72298</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
-        <v>44989</v>
+        <v>44991</v>
       </c>
       <c r="B67" s="12">
-        <v>60348</v>
+        <v>69721</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
-        <v>44990</v>
+        <v>44992</v>
       </c>
       <c r="B68" s="2">
-        <v>72298</v>
+        <v>61125</v>
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B69" s="12">
-        <v>69721</v>
+        <v>79270</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="B70" s="2">
-        <v>61125</v>
+        <v>45347</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
-        <v>44993</v>
+        <v>44995</v>
       </c>
       <c r="B71" s="12">
-        <v>79270</v>
+        <v>46243</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
-        <v>44994</v>
+        <v>44996</v>
       </c>
       <c r="B72" s="2">
-        <v>45347</v>
+        <v>77384</v>
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
-        <v>44995</v>
+        <v>44997</v>
       </c>
       <c r="B73" s="12">
-        <v>46243</v>
+        <v>55917</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
-        <v>44996</v>
+        <v>44998</v>
       </c>
       <c r="B74" s="2">
-        <v>77384</v>
+        <v>57507</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
-        <v>44997</v>
+        <v>44999</v>
       </c>
       <c r="B75" s="12">
-        <v>55917</v>
+        <v>53797</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
-        <v>44998</v>
+        <v>45000</v>
       </c>
       <c r="B76" s="2">
-        <v>57507</v>
+        <v>73461</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
-        <v>44999</v>
+        <v>45001</v>
       </c>
       <c r="B77" s="12">
-        <v>53797</v>
+        <v>45694</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
-        <v>45000</v>
+        <v>45002</v>
       </c>
       <c r="B78" s="2">
-        <v>73461</v>
+        <v>61866</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
-        <v>45001</v>
+        <v>45003</v>
       </c>
       <c r="B79" s="12">
-        <v>45694</v>
+        <v>33286</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
-        <v>45002</v>
+        <v>45004</v>
       </c>
       <c r="B80" s="2">
-        <v>61866</v>
+        <v>31087</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
-        <v>45003</v>
+        <v>45005</v>
       </c>
       <c r="B81" s="12">
-        <v>33286</v>
+        <v>52874</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
-        <v>45004</v>
+        <v>45006</v>
       </c>
       <c r="B82" s="2">
-        <v>31087</v>
+        <v>39942</v>
       </c>
       <c r="E82" s="9"/>
       <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
-        <v>45005</v>
+        <v>45007</v>
       </c>
       <c r="B83" s="12">
-        <v>52874</v>
+        <v>59000</v>
       </c>
       <c r="E83" s="9"/>
       <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
-        <v>45006</v>
+        <v>45008</v>
       </c>
       <c r="B84" s="2">
-        <v>39942</v>
+        <v>51423</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
-        <v>45007</v>
+        <v>45009</v>
       </c>
       <c r="B85" s="12">
-        <v>59000</v>
+        <v>57857</v>
       </c>
       <c r="E85" s="9"/>
       <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
-        <v>45008</v>
+        <v>45010</v>
       </c>
       <c r="B86" s="2">
-        <v>51423</v>
+        <v>76193</v>
       </c>
       <c r="E86" s="9"/>
       <c r="F86" s="2"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
-        <v>45009</v>
+        <v>45011</v>
       </c>
       <c r="B87" s="12">
-        <v>57857</v>
+        <v>70551</v>
       </c>
       <c r="E87" s="9"/>
       <c r="F87" s="2"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
-        <v>45010</v>
+        <v>45012</v>
       </c>
       <c r="B88" s="2">
-        <v>76193</v>
+        <v>74145</v>
       </c>
       <c r="E88" s="9"/>
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
-        <v>45011</v>
+        <v>45013</v>
       </c>
       <c r="B89" s="12">
-        <v>70551</v>
+        <v>79181</v>
       </c>
       <c r="E89" s="9"/>
       <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
-        <v>45012</v>
+        <v>45014</v>
       </c>
       <c r="B90" s="2">
-        <v>74145</v>
+        <v>63917</v>
       </c>
       <c r="E90" s="9"/>
       <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
-        <v>45013</v>
+        <v>45015</v>
       </c>
       <c r="B91" s="12">
-        <v>79181</v>
+        <v>74700</v>
       </c>
       <c r="E91" s="9"/>
       <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
-        <v>45014</v>
+        <v>45016</v>
       </c>
       <c r="B92" s="2">
-        <v>63917</v>
+        <v>71584</v>
       </c>
       <c r="E92" s="9"/>
       <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="9">
-        <v>45015</v>
-      </c>
-      <c r="B93" s="12">
-        <v>74700</v>
-      </c>
-      <c r="E93" s="9"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="9">
-        <v>45016</v>
-      </c>
-      <c r="B94" s="2">
-        <v>71584</v>
-      </c>
-      <c r="E94" s="9"/>
-      <c r="F94" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="I4:S4"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{ED186D72-9B71-9848-AD32-86ECB806C3AE}">
-      <formula1>$S$3:$S$6</formula1>
+      <formula1>_xlfn.ANCHORARRAY($I$6)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>